<commit_message>
Edit database in excel (Promotion)
</commit_message>
<xml_diff>
--- a/Database/Quick-Look-Database.xlsx
+++ b/Database/Quick-Look-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Intern-CFOX\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5357CCB5-66D9-4A9B-8D94-BE045073076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C351A5C3-066A-4A4C-9E9C-532192951A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{400451B1-2A96-4ACF-9895-274AFC7C227C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{400451B1-2A96-4ACF-9895-274AFC7C227C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>NOT NULL, &gt; 10,000</t>
+  </si>
+  <si>
+    <t>NOT NULL, &gt; start_date</t>
   </si>
 </sst>
 </file>
@@ -557,6 +560,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,9 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -894,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7947285-B6E9-4448-9972-18FAB4849A0C}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,14 +914,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1087,14 +1090,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1265,14 +1268,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1333,14 +1336,14 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1430,7 +1433,7 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>62</v>
@@ -1491,14 +1494,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -1595,14 +1598,14 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
@@ -1769,14 +1772,14 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -1809,7 +1812,7 @@
         <v>79</v>
       </c>
       <c r="D58" s="3"/>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -1827,7 +1830,7 @@
         <v>23</v>
       </c>
       <c r="D59" s="3"/>
-      <c r="E59" s="13"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="3" t="s">
         <v>24</v>
       </c>
@@ -1873,14 +1876,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="E58:E59"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A28:F28"/>
     <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="E58:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update datebase for promotion
</commit_message>
<xml_diff>
--- a/Database/Quick-Look-Database.xlsx
+++ b/Database/Quick-Look-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Intern-CFOX\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C351A5C3-066A-4A4C-9E9C-532192951A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474BA7BD-9525-407E-A937-07BFB078C0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{400451B1-2A96-4ACF-9895-274AFC7C227C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{400451B1-2A96-4ACF-9895-274AFC7C227C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>NOT NULL, &gt; start_date</t>
+  </si>
+  <si>
+    <t>FK</t>
   </si>
 </sst>
 </file>
@@ -560,12 +563,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,11 +572,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7947285-B6E9-4448-9972-18FAB4849A0C}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,14 +917,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1090,14 +1093,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1268,14 +1271,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1336,14 +1339,14 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1494,14 +1497,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -1598,14 +1601,14 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
@@ -1675,7 +1678,7 @@
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>55</v>
@@ -1772,14 +1775,14 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -1812,7 +1815,7 @@
         <v>79</v>
       </c>
       <c r="D58" s="3"/>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="12" t="s">
         <v>94</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -1830,7 +1833,7 @@
         <v>23</v>
       </c>
       <c r="D59" s="3"/>
-      <c r="E59" s="14"/>
+      <c r="E59" s="13"/>
       <c r="F59" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Update note for status in Order
</commit_message>
<xml_diff>
--- a/Database/Quick-Look-Database.xlsx
+++ b/Database/Quick-Look-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Intern-CFOX\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474BA7BD-9525-407E-A937-07BFB078C0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63EB8C0-FAA4-4ACC-B749-60205DEC162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{400451B1-2A96-4ACF-9895-274AFC7C227C}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>Trạng thái đơn hàng</t>
-  </si>
-  <si>
     <t>Ghi chú (optional)</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>Trạng thái đơn hàng (0 là đang gặp vấn đề, 1 là hoàn thành, 2 là đã xử lý lỗi) có thể bổ sung nhiều trạng thái sau đó</t>
   </si>
 </sst>
 </file>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7947285-B6E9-4448-9972-18FAB4849A0C}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +911,7 @@
     <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -976,7 +976,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
@@ -1007,17 +1007,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,14 +1028,14 @@
         <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>33</v>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>37</v>
@@ -1242,14 +1242,14 @@
         <v>38</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>52</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>62</v>
@@ -1450,7 +1450,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
@@ -1468,11 +1468,11 @@
         <v>40</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>66</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>67</v>
@@ -1572,11 +1572,11 @@
         <v>73</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>74</v>
@@ -1587,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>55</v>
@@ -1710,7 +1710,7 @@
         <v>85</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
@@ -1735,7 +1735,7 @@
         <v>18</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1761,22 +1761,22 @@
         <v>8</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>81</v>
@@ -1853,7 +1853,7 @@
         <v>36</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,17 +1864,17 @@
         <v>38</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>